<commit_message>
Amended Mean function and test script (one error to resolve with test script)
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Mean.xlsx
+++ b/tests/testthat/testdata_Mean.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
   <si>
     <t>Area1</t>
   </si>
@@ -33,27 +33,9 @@
     <t>Area2</t>
   </si>
   <si>
-    <t>lower95cl</t>
-  </si>
-  <si>
-    <t>upper95cl</t>
-  </si>
-  <si>
-    <t>lower998cl</t>
-  </si>
-  <si>
-    <t>upper998cl</t>
-  </si>
-  <si>
     <t>stdev</t>
   </si>
   <si>
-    <t>numrecs</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
@@ -64,6 +46,36 @@
   </si>
   <si>
     <t>No grouping</t>
+  </si>
+  <si>
+    <t>lowercl</t>
+  </si>
+  <si>
+    <t>uppercl</t>
+  </si>
+  <si>
+    <t>confidence</t>
+  </si>
+  <si>
+    <t>statistic</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>99.8%</t>
+  </si>
+  <si>
+    <t>Student's t-distribution</t>
+  </si>
+  <si>
+    <t>value_sum</t>
+  </si>
+  <si>
+    <t>value_count</t>
   </si>
 </sst>
 </file>
@@ -113,11 +125,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,7 +415,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B27"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,10 +428,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,50 +658,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="5"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -698,10 +717,10 @@
         <v>8</v>
       </c>
       <c r="D2">
+        <v>20.975575257709309</v>
+      </c>
+      <c r="E2">
         <v>53.704345000000011</v>
-      </c>
-      <c r="E2">
-        <v>20.975575257709309</v>
       </c>
       <c r="F2">
         <v>36.168325241336504</v>
@@ -709,14 +728,17 @@
       <c r="G2">
         <v>71.240364758663517</v>
       </c>
-      <c r="H2">
-        <v>18.216705294788838</v>
-      </c>
-      <c r="I2">
-        <v>89.191984705211183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -727,10 +749,10 @@
         <v>18</v>
       </c>
       <c r="D3">
+        <v>2117.8317161590671</v>
+      </c>
+      <c r="E3">
         <v>5678.9629577777778</v>
-      </c>
-      <c r="E3">
-        <v>2117.8317161590671</v>
       </c>
       <c r="F3">
         <v>4625.7900224529722</v>
@@ -738,16 +760,19 @@
       <c r="G3">
         <v>6732.1358931025834</v>
       </c>
-      <c r="H3">
-        <v>3859.0770997295967</v>
-      </c>
-      <c r="I3">
-        <v>7498.8488158259588</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <f>SUM(B2:B3)</f>
@@ -758,10 +783,10 @@
         <v>26</v>
       </c>
       <c r="D4">
+        <v>3171.8018122194453</v>
+      </c>
+      <c r="E4">
         <v>3948.1141538461534</v>
-      </c>
-      <c r="E4">
-        <v>3171.8018122194453</v>
       </c>
       <c r="F4">
         <v>2666.9956767458489</v>
@@ -769,11 +794,112 @@
       <c r="G4">
         <v>5229.2326309464579</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>429.63476000000009</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>20.975575257709309</v>
+      </c>
+      <c r="E5">
+        <v>53.704345000000011</v>
+      </c>
+      <c r="F5">
+        <v>18.216705294788838</v>
+      </c>
+      <c r="G5">
+        <v>89.191984705211183</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>102221.33323999999</v>
+      </c>
+      <c r="C6">
+        <v>18</v>
+      </c>
+      <c r="D6">
+        <v>2117.8317161590671</v>
+      </c>
+      <c r="E6">
+        <v>5678.9629577777778</v>
+      </c>
+      <c r="F6">
+        <v>3859.0770997295967</v>
+      </c>
+      <c r="G6">
+        <v>7498.8488158259588</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f>SUM(B5:B6)</f>
+        <v>102650.96799999999</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C5:C6)</f>
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>3171.8018122194453</v>
+      </c>
+      <c r="E7">
+        <v>3948.1141538461534</v>
+      </c>
+      <c r="F7">
         <v>1801.9535385474737</v>
       </c>
-      <c r="I4">
+      <c r="G7">
         <v>6094.274769144833</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Amended Mean, Proportion and Rate test scripts.  Amended DSR vignette (WIP).
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Mean.xlsx
+++ b/tests/testthat/testdata_Mean.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>Area1</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>value_count</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added testing to imporve coverage for 2-CI functionality.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata_Mean.xlsx
+++ b/tests/testthat/testdata_Mean.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEstatmethods\tests\testthat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georgina.Anderson\Documents\R\Projects\PHEindicatormethods\tests\testthat\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7739ECCC-129B-45F1-9497-E479995926D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testdata_Mean" sheetId="3" r:id="rId1"/>
     <sheet name="testdata_Mean_results" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
   <si>
     <t>Area1</t>
   </si>
@@ -48,27 +49,12 @@
     <t>No grouping</t>
   </si>
   <si>
-    <t>lowercl</t>
-  </si>
-  <si>
-    <t>uppercl</t>
-  </si>
-  <si>
-    <t>confidence</t>
-  </si>
-  <si>
     <t>statistic</t>
   </si>
   <si>
     <t>method</t>
   </si>
   <si>
-    <t>95%</t>
-  </si>
-  <si>
-    <t>99.8%</t>
-  </si>
-  <si>
     <t>Student's t-distribution</t>
   </si>
   <si>
@@ -79,12 +65,24 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>lower99_8cl</t>
+  </si>
+  <si>
+    <t>upper99_8cl</t>
+  </si>
+  <si>
+    <t>lower95_0cl</t>
+  </si>
+  <si>
+    <t>upper95_0cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,13 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -660,11 +656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -673,43 +669,46 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="5"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -731,17 +730,20 @@
       <c r="G2">
         <v>71.240364758663517</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H2">
+        <v>18.216705294788838</v>
+      </c>
+      <c r="I2">
+        <v>89.191984705211183</v>
+      </c>
+      <c r="J2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -763,17 +765,20 @@
       <c r="G3">
         <v>6732.1358931025834</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="H3">
+        <v>3859.0770997295967</v>
+      </c>
+      <c r="I3">
+        <v>7498.8488158259588</v>
+      </c>
+      <c r="J3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -797,112 +802,17 @@
       <c r="G4">
         <v>5229.2326309464579</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="H4">
+        <v>1801.9535385474737</v>
+      </c>
+      <c r="I4">
+        <v>6094.274769144833</v>
+      </c>
+      <c r="J4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>429.63476000000009</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>20.975575257709309</v>
-      </c>
-      <c r="E5">
-        <v>53.704345000000011</v>
-      </c>
-      <c r="F5">
-        <v>18.216705294788838</v>
-      </c>
-      <c r="G5">
-        <v>89.191984705211183</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>102221.33323999999</v>
-      </c>
-      <c r="C6">
-        <v>18</v>
-      </c>
-      <c r="D6">
-        <v>2117.8317161590671</v>
-      </c>
-      <c r="E6">
-        <v>5678.9629577777778</v>
-      </c>
-      <c r="F6">
-        <v>3859.0770997295967</v>
-      </c>
-      <c r="G6">
-        <v>7498.8488158259588</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f>SUM(B5:B6)</f>
-        <v>102650.96799999999</v>
-      </c>
-      <c r="C7">
-        <f>SUM(C5:C6)</f>
-        <v>26</v>
-      </c>
-      <c r="D7">
-        <v>3171.8018122194453</v>
-      </c>
-      <c r="E7">
-        <v>3948.1141538461534</v>
-      </c>
-      <c r="F7">
-        <v>1801.9535385474737</v>
-      </c>
-      <c r="G7">
-        <v>6094.274769144833</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" t="s">
-        <v>14</v>
+      <c r="K4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>